<commit_message>
Downloader: Fix a crash in the download function
`Throwable.initCause` throws an IllegalStateException in case a cause has
already been set. As the download function calls `initCause` on the exception
caught from `downloadSourceArtifact`, which in turn can throw exceptions with a
cause already set, the downloader runs into that problem.

Fix this by using `Throwable.addSuppressedException` instead of
`Throwable.initCause` which seems also more suitable for accumulating multiple
exceptions originating from sibling code of the call tree.

Signed-off-by: Frank Viernau <frank.viernau@here.com>
</commit_message>
<xml_diff>
--- a/reporter/src/funTest/assets/file-counter-expected-scan-report.xlsx
+++ b/reporter/src/funTest/assets/file-counter-expected-scan-report.xlsx
@@ -98,8 +98,9 @@
         <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Gradle:com.here.ort.gradle.example:lib:1.0.0
-  Unknown time [ERROR]: FileCounter - DownloadException: No source artifact URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'.
-Caused by: DownloadException: No VCS URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'. Please make sure the release POM file includes the SCM connection, see: https://docs.gradle.org/current/userguide/publishing_maven.html#example_customizing_the_pom_file
+  Unknown time [ERROR]: FileCounter - DownloadException: Download failed for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'.
+Suppressed: DownloadException: No VCS URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'. Please make sure the release POM file includes the SCM connection, see: https://docs.gradle.org/current/userguide/publishing_maven.html#example_customizing_the_pom_file, 
+Suppressed: DownloadException: No source artifact URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'.
 </t>
     </r>
   </si>
@@ -222,8 +223,9 @@
         <sz val="11.0"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>Unknown time [ERROR]: FileCounter - DownloadException: No source artifact URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'.
-Caused by: DownloadException: No VCS URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'. Please make sure the release POM file includes the SCM connection, see: https://docs.gradle.org/current/userguide/publishing_maven.html#example_customizing_the_pom_file</t>
+      <t>Unknown time [ERROR]: FileCounter - DownloadException: Download failed for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'.
+Suppressed: DownloadException: No VCS URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'. Please make sure the release POM file includes the SCM connection, see: https://docs.gradle.org/current/userguide/publishing_maven.html#example_customizing_the_pom_file, 
+Suppressed: DownloadException: No source artifact URL provided for 'Gradle:com.here.ort.gradle.example:lib:1.0.0'.</t>
     </r>
   </si>
   <si>

</xml_diff>